<commit_message>
more cleanup of the files
</commit_message>
<xml_diff>
--- a/ref/CMU_English_Phonemes.xlsx
+++ b/ref/CMU_English_Phonemes.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="162">
   <si>
     <t>English Phoneme</t>
   </si>
@@ -306,6 +306,9 @@
   </si>
   <si>
     <t>P</t>
+  </si>
+  <si>
+    <t>N-G</t>
   </si>
   <si>
     <t>PeN-G</t>
@@ -685,8 +688,8 @@
   </sheetPr>
   <dimension ref="A1:S47"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I13" activeCellId="0" sqref="I13"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L25" activeCellId="0" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1376,11 +1379,14 @@
       <c r="G25" s="0" t="s">
         <v>93</v>
       </c>
+      <c r="K25" s="0" t="s">
+        <v>96</v>
+      </c>
       <c r="L25" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="M25" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="N25" s="0" t="s">
         <v>96</v>
@@ -1389,7 +1395,7 @@
         <v>38</v>
       </c>
       <c r="P25" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="Q25" s="0" t="s">
         <v>66</v>
@@ -1397,28 +1403,28 @@
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D26" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E26" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="G26" s="0" t="s">
         <v>100</v>
       </c>
-      <c r="G26" s="0" t="s">
-        <v>99</v>
-      </c>
       <c r="H26" s="0" t="s">
         <v>13</v>
       </c>
       <c r="L26" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="M26" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="N26" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="N26" s="0" t="s">
-        <v>101</v>
-      </c>
       <c r="O26" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="P26" s="0" t="s">
         <v>13</v>
@@ -1426,31 +1432,31 @@
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D27" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E27" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="G27" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H27" s="0" t="s">
         <v>105</v>
       </c>
-      <c r="G27" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H27" s="0" t="s">
-        <v>104</v>
-      </c>
       <c r="L27" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="M27" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="N27" s="0" t="s">
         <v>13</v>
       </c>
       <c r="O27" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="P27" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1458,7 +1464,7 @@
         <v>96</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="G28" s="0" t="s">
         <v>96</v>
@@ -1470,7 +1476,7 @@
         <v>96</v>
       </c>
       <c r="M28" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="N28" s="0" t="s">
         <v>96</v>
@@ -1484,7 +1490,7 @@
         <v>68</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G29" s="0" t="s">
         <v>68</v>
@@ -1499,7 +1505,7 @@
         <v>68</v>
       </c>
       <c r="M29" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="N29" s="0" t="s">
         <v>68</v>
@@ -1513,25 +1519,25 @@
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D30" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E30" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="G30" s="0" t="s">
         <v>115</v>
       </c>
-      <c r="G30" s="0" t="s">
-        <v>114</v>
-      </c>
       <c r="H30" s="0" t="s">
         <v>36</v>
       </c>
       <c r="L30" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="M30" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="N30" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="O30" s="0" t="s">
         <v>44</v>
@@ -1539,25 +1545,25 @@
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D31" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E31" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="G31" s="0" t="s">
         <v>118</v>
       </c>
-      <c r="G31" s="0" t="s">
-        <v>117</v>
-      </c>
       <c r="H31" s="0" t="s">
         <v>36</v>
       </c>
       <c r="L31" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="M31" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="N31" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="O31" s="0" t="s">
         <v>19</v>
@@ -1571,7 +1577,7 @@
         <v>13</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="G32" s="0" t="s">
         <v>13</v>
@@ -1583,7 +1589,7 @@
         <v>13</v>
       </c>
       <c r="M32" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="N32" s="0" t="s">
         <v>13</v>
@@ -1594,13 +1600,13 @@
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D33" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E33" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="G33" s="0" t="s">
         <v>125</v>
-      </c>
-      <c r="G33" s="0" t="s">
-        <v>124</v>
       </c>
       <c r="H33" s="0" t="s">
         <v>59</v>
@@ -1612,13 +1618,13 @@
         <v>16</v>
       </c>
       <c r="L33" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="M33" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="N33" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="O33" s="0" t="s">
         <v>19</v>
@@ -1630,39 +1636,39 @@
         <v>13</v>
       </c>
       <c r="R33" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D34" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="G34" s="0" t="s">
         <v>18</v>
       </c>
       <c r="H34" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="I34" s="0" t="s">
         <v>7</v>
       </c>
       <c r="L34" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="M34" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="N34" s="0" t="s">
         <v>19</v>
       </c>
       <c r="O34" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="P34" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="Q34" s="0" t="s">
         <v>7</v>
@@ -1670,51 +1676,51 @@
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D35" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E35" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="F35" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G35" s="0" t="s">
         <v>136</v>
       </c>
-      <c r="F35" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="G35" s="0" t="s">
-        <v>135</v>
-      </c>
       <c r="L35" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="M35" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="N35" s="0" t="s">
         <v>13</v>
       </c>
       <c r="O35" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D36" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E36" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="G36" s="0" t="s">
         <v>139</v>
       </c>
-      <c r="G36" s="0" t="s">
-        <v>138</v>
-      </c>
       <c r="H36" s="0" t="s">
         <v>36</v>
       </c>
       <c r="L36" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="M36" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="N36" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="O36" s="0" t="s">
         <v>44</v>
@@ -1722,25 +1728,25 @@
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D37" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="E37" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="G37" s="0" t="s">
         <v>142</v>
       </c>
-      <c r="G37" s="0" t="s">
-        <v>141</v>
-      </c>
       <c r="H37" s="0" t="s">
         <v>36</v>
       </c>
       <c r="L37" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="M37" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="N37" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="O37" s="0" t="s">
         <v>38</v>
@@ -1748,13 +1754,13 @@
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D38" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="G38" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="H38" s="0" t="s">
         <v>36</v>
@@ -1766,19 +1772,19 @@
         <v>7</v>
       </c>
       <c r="L38" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="M38" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="N38" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="O38" s="0" t="s">
         <v>44</v>
       </c>
       <c r="P38" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="Q38" s="0" t="s">
         <v>7</v>
@@ -1789,7 +1795,7 @@
         <v>41</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="G39" s="0" t="s">
         <v>41</v>
@@ -1801,7 +1807,7 @@
         <v>41</v>
       </c>
       <c r="M39" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="N39" s="0" t="s">
         <v>41</v>
@@ -1812,40 +1818,40 @@
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D40" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E40" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="F40" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="G40" s="0" t="s">
         <v>150</v>
-      </c>
-      <c r="F40" s="0" t="s">
-        <v>151</v>
-      </c>
-      <c r="G40" s="0" t="s">
-        <v>149</v>
       </c>
       <c r="H40" s="0" t="s">
         <v>55</v>
       </c>
       <c r="L40" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="M40" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="N40" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="O40" s="0" t="s">
         <v>44</v>
       </c>
       <c r="P40" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="Q40" s="0" t="s">
         <v>19</v>
       </c>
       <c r="R40" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="S40" s="0" t="s">
         <v>68</v>
@@ -1853,32 +1859,32 @@
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>

</xml_diff>